<commit_message>
update the db idea
</commit_message>
<xml_diff>
--- a/final_project/db_design.xlsx
+++ b/final_project/db_design.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC09D3B-6A52-418C-9DFB-5CB50F8BC698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C977B492-8957-4122-9D18-10EAF1613812}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="4" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
     <sheet name="Courses" sheetId="3" r:id="rId2"/>
     <sheet name="Fields of study" sheetId="2" r:id="rId3"/>
-    <sheet name="Instructors" sheetId="4" r:id="rId4"/>
+    <sheet name="Grades" sheetId="5" r:id="rId4"/>
+    <sheet name="Instructors" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>Index</t>
   </si>
@@ -252,18 +253,12 @@
     <t>AIR</t>
   </si>
   <si>
-    <t>CBE</t>
-  </si>
-  <si>
     <t>Electornic and Computer Engineering</t>
   </si>
   <si>
     <t>Automatyka i Robotyka</t>
   </si>
   <si>
-    <t>Cyberbezpieczeństwo</t>
-  </si>
-  <si>
     <t>ECTS deficit</t>
   </si>
   <si>
@@ -304,12 +299,30 @@
   </si>
   <si>
     <t>Robak</t>
+  </si>
+  <si>
+    <t>TIN</t>
+  </si>
+  <si>
+    <t>Teleinformatyka</t>
+  </si>
+  <si>
+    <t>Course_ID</t>
+  </si>
+  <si>
+    <t>Student_ID</t>
+  </si>
+  <si>
+    <t>Grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -392,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,6 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4C6B96-C4DC-4735-B81E-35A8CA1960AC}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -760,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1284,13 +1298,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1301,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1312,10 +1328,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1326,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1340,10 +1356,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1354,10 +1370,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1368,10 +1384,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1387,7 +1403,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1416,7 +1432,7 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1427,7 +1443,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1435,10 +1451,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1452,16 +1468,68 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7C17CB-17CC-4531-A19C-16586065C374}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BBAA83-CB17-480D-9BF2-9E6FB44F98AF}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7C17CB-17CC-4531-A19C-16586065C374}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1480,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1491,10 +1559,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1502,10 +1570,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1513,10 +1581,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final project, project
</commit_message>
<xml_diff>
--- a/final_project/db_design.xlsx
+++ b/final_project/db_design.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C977B492-8957-4122-9D18-10EAF1613812}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778F371F-2CB1-4703-834A-18D24502065C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="4" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
     <sheet name="Courses" sheetId="3" r:id="rId2"/>
     <sheet name="Fields of study" sheetId="2" r:id="rId3"/>
     <sheet name="Grades" sheetId="5" r:id="rId4"/>
-    <sheet name="Instructors" sheetId="4" r:id="rId5"/>
+    <sheet name="Grades comments" sheetId="8" r:id="rId5"/>
+    <sheet name="Suspended students" sheetId="9" r:id="rId6"/>
+    <sheet name="Instructors" sheetId="4" r:id="rId7"/>
+    <sheet name="Enrollments" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Index</t>
   </si>
@@ -314,6 +317,24 @@
   </si>
   <si>
     <t>Grade</t>
+  </si>
+  <si>
+    <t>Student_Index</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Grade_ID</t>
+  </si>
+  <si>
+    <t>Some comment.</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Some reason…</t>
   </si>
 </sst>
 </file>
@@ -321,9 +342,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,11 +767,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4C6B96-C4DC-4735-B81E-35A8CA1960AC}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
@@ -760,7 +781,7 @@
     <col min="10" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100100</v>
       </c>
@@ -794,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100101</v>
       </c>
@@ -811,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100102</v>
       </c>
@@ -828,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100103</v>
       </c>
@@ -845,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100104</v>
       </c>
@@ -862,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>100105</v>
       </c>
@@ -879,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100106</v>
       </c>
@@ -896,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>100107</v>
       </c>
@@ -913,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100108</v>
       </c>
@@ -930,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100109</v>
       </c>
@@ -947,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>100110</v>
       </c>
@@ -964,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>100111</v>
       </c>
@@ -981,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100112</v>
       </c>
@@ -998,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>100113</v>
       </c>
@@ -1015,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>100114</v>
       </c>
@@ -1032,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>100115</v>
       </c>
@@ -1049,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>100116</v>
       </c>
@@ -1066,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>100117</v>
       </c>
@@ -1083,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>100118</v>
       </c>
@@ -1100,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>100119</v>
       </c>
@@ -1117,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>100120</v>
       </c>
@@ -1134,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100121</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>100122</v>
       </c>
@@ -1168,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>100123</v>
       </c>
@@ -1185,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>100124</v>
       </c>
@@ -1202,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>100125</v>
       </c>
@@ -1219,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100126</v>
       </c>
@@ -1236,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>100127</v>
       </c>
@@ -1253,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>100128</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>100129</v>
       </c>
@@ -1298,10 +1319,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -1309,7 +1330,7 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1323,9 +1344,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -1337,9 +1358,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
@@ -1351,9 +1372,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
@@ -1365,9 +1386,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
@@ -1379,9 +1400,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
@@ -1406,14 +1427,14 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1435,7 +1456,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1446,7 +1467,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1457,7 +1478,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1472,10 +1493,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
@@ -1483,7 +1504,7 @@
     <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1505,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>100101</v>
       </c>
       <c r="D2" s="8">
         <v>4</v>
@@ -1518,21 +1539,90 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8ECDD-6B59-425A-9189-E22DC1282E23}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13B9986-6B44-407B-9E7B-E5C69B4870CC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7C17CB-17CC-4531-A19C-16586065C374}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1543,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1554,7 +1644,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1565,7 +1655,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1576,7 +1666,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1585,6 +1675,48 @@
       </c>
       <c r="C5" t="s">
         <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAC7ABB-2671-49BC-9122-B2CF83A2CAC4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use std::vector instead of std::unordered_map for columns
</commit_message>
<xml_diff>
--- a/final_project/db_design.xlsx
+++ b/final_project/db_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94D2C597-E819-4045-BDEE-FE06C81708DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8873F76D-EC4A-40C6-995C-E0052EB822F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="-120" windowWidth="27975" windowHeight="16440" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Some reason…</t>
   </si>
   <si>
-    <t>Field _of_study</t>
-  </si>
-  <si>
     <t>ECTS_deficit</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>Full_name</t>
+  </si>
+  <si>
+    <t>Field_of_study</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,10 +792,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1439,10 +1439,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>